<commit_message>
fixes: xls files, remove comments
</commit_message>
<xml_diff>
--- a/WebApp/survey_data.xlsx
+++ b/WebApp/survey_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ye.xu2\Ye\Personal\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianjohnson/Desktop/Columbia/maudson-nlp/Capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11220" windowHeight="3465"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Women's Informational Survey Hi" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,15 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Women''s Informational Survey Hi'!$A$1:$H$457</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -7704,9 +7712,6 @@
     <t>cleaning your body</t>
   </si>
   <si>
-    <t>What is Healthy Skin?</t>
-  </si>
-  <si>
     <t xml:space="preserve">How do you get healthy skin?
 </t>
   </si>
@@ -7723,6 +7728,9 @@
   <si>
     <t xml:space="preserve">How do you know your skin is getting healthier with every shower?
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is Healthy " ' … , ' " Skin? </t>
   </si>
 </sst>
 </file>
@@ -7875,9 +7883,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -7910,9 +7918,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -8118,45 +8126,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="43.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="43.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2552</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2556</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2557</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2553</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2555</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2554</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>33839</v>
       </c>
@@ -8182,7 +8190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>36761</v>
       </c>
@@ -8208,7 +8216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>6756</v>
       </c>
@@ -8234,7 +8242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>16468</v>
       </c>
@@ -8260,7 +8268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>11551</v>
       </c>
@@ -8286,7 +8294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>8548</v>
       </c>
@@ -8312,7 +8320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>21768</v>
       </c>
@@ -8338,7 +8346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>22278</v>
       </c>
@@ -8364,7 +8372,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2210</v>
       </c>
@@ -8390,7 +8398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>24401</v>
       </c>
@@ -8416,7 +8424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>13877</v>
       </c>
@@ -8442,7 +8450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>8355</v>
       </c>
@@ -8468,7 +8476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>29899</v>
       </c>
@@ -8494,7 +8502,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>27837</v>
       </c>
@@ -8520,7 +8528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>36854</v>
       </c>
@@ -8546,7 +8554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>35063</v>
       </c>
@@ -8572,7 +8580,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1869</v>
       </c>
@@ -8598,7 +8606,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>8010</v>
       </c>
@@ -8624,7 +8632,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>827</v>
       </c>
@@ -8650,7 +8658,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>33779</v>
       </c>
@@ -8676,7 +8684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>9532</v>
       </c>
@@ -8702,7 +8710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>12750</v>
       </c>
@@ -8728,7 +8736,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>12002</v>
       </c>
@@ -8754,7 +8762,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>36188</v>
       </c>
@@ -8780,7 +8788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7112</v>
       </c>
@@ -8806,7 +8814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>772</v>
       </c>
@@ -8832,7 +8840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1235</v>
       </c>
@@ -8858,7 +8866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>33845</v>
       </c>
@@ -8884,7 +8892,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>24044</v>
       </c>
@@ -8910,7 +8918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28775</v>
       </c>
@@ -8936,7 +8944,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>10301</v>
       </c>
@@ -8962,7 +8970,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>10070</v>
       </c>
@@ -8988,7 +8996,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>27818</v>
       </c>
@@ -9014,7 +9022,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>6238</v>
       </c>
@@ -9040,7 +9048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>32129</v>
       </c>
@@ -9066,7 +9074,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>5207</v>
       </c>
@@ -9092,7 +9100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>31692</v>
       </c>
@@ -9118,7 +9126,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>35165</v>
       </c>
@@ -9144,7 +9152,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>21802</v>
       </c>
@@ -9170,7 +9178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2269</v>
       </c>
@@ -9196,7 +9204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1852</v>
       </c>
@@ -9222,7 +9230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>5818</v>
       </c>
@@ -9248,7 +9256,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>707</v>
       </c>
@@ -9274,7 +9282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>519</v>
       </c>
@@ -9300,7 +9308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>22364</v>
       </c>
@@ -9326,7 +9334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>36759</v>
       </c>
@@ -9352,7 +9360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>9582</v>
       </c>
@@ -9378,7 +9386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>13139</v>
       </c>
@@ -9404,7 +9412,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>36112</v>
       </c>
@@ -9430,7 +9438,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>5356</v>
       </c>
@@ -9456,7 +9464,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>4046</v>
       </c>
@@ -9482,7 +9490,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>2336</v>
       </c>
@@ -9508,7 +9516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>34426</v>
       </c>
@@ -9534,7 +9542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>6237</v>
       </c>
@@ -9560,7 +9568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>36227</v>
       </c>
@@ -9586,7 +9594,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>15890</v>
       </c>
@@ -9612,7 +9620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>26658</v>
       </c>
@@ -9638,7 +9646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>8575</v>
       </c>
@@ -9664,7 +9672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>31914</v>
       </c>
@@ -9690,7 +9698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>8761</v>
       </c>
@@ -9716,7 +9724,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2110</v>
       </c>
@@ -9742,7 +9750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>35958</v>
       </c>
@@ -9768,7 +9776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>36629</v>
       </c>
@@ -9794,7 +9802,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>8400</v>
       </c>
@@ -9820,7 +9828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>7975</v>
       </c>
@@ -9846,7 +9854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>16186</v>
       </c>
@@ -9872,7 +9880,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>4756</v>
       </c>
@@ -9898,7 +9906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>10420</v>
       </c>
@@ -9924,7 +9932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>26010</v>
       </c>
@@ -9950,7 +9958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>35200</v>
       </c>
@@ -9976,7 +9984,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>1783</v>
       </c>
@@ -10002,7 +10010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>27215</v>
       </c>
@@ -10028,7 +10036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>33755</v>
       </c>
@@ -10054,7 +10062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>19021</v>
       </c>
@@ -10080,7 +10088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>36581</v>
       </c>
@@ -10106,7 +10114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>6332</v>
       </c>
@@ -10132,7 +10140,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>22001</v>
       </c>
@@ -10158,7 +10166,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>274</v>
       </c>
@@ -10184,7 +10192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>16493</v>
       </c>
@@ -10210,7 +10218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>34469</v>
       </c>
@@ -10236,7 +10244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>24385</v>
       </c>
@@ -10262,7 +10270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>35355</v>
       </c>
@@ -10288,7 +10296,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>21699</v>
       </c>
@@ -10314,7 +10322,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>16521</v>
       </c>
@@ -10340,7 +10348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>34901</v>
       </c>
@@ -10366,7 +10374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>18736</v>
       </c>
@@ -10392,7 +10400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>1397</v>
       </c>
@@ -10418,7 +10426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>10904</v>
       </c>
@@ -10444,7 +10452,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>16519</v>
       </c>
@@ -10470,7 +10478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>6066</v>
       </c>
@@ -10496,7 +10504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>32097</v>
       </c>
@@ -10522,7 +10530,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>18890</v>
       </c>
@@ -10548,7 +10556,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>36708</v>
       </c>
@@ -10574,7 +10582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>912</v>
       </c>
@@ -10600,7 +10608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>26149</v>
       </c>
@@ -10626,7 +10634,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>12737</v>
       </c>
@@ -10652,7 +10660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>15621</v>
       </c>
@@ -10678,7 +10686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>34731</v>
       </c>
@@ -10704,7 +10712,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>28761</v>
       </c>
@@ -10730,7 +10738,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>2524</v>
       </c>
@@ -10756,7 +10764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>34928</v>
       </c>
@@ -10782,7 +10790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>5643</v>
       </c>
@@ -10808,7 +10816,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>22419</v>
       </c>
@@ -10834,7 +10842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>8280</v>
       </c>
@@ -10860,7 +10868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>23691</v>
       </c>
@@ -10886,7 +10894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>8570</v>
       </c>
@@ -10912,7 +10920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>18469</v>
       </c>
@@ -10938,7 +10946,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>33616</v>
       </c>
@@ -10964,7 +10972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>7545</v>
       </c>
@@ -10990,7 +10998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>13288</v>
       </c>
@@ -11016,7 +11024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>36038</v>
       </c>
@@ -11042,7 +11050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>36927</v>
       </c>
@@ -11068,7 +11076,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>1195</v>
       </c>
@@ -11094,7 +11102,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>32983</v>
       </c>
@@ -11120,7 +11128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>36858</v>
       </c>
@@ -11146,7 +11154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>24622</v>
       </c>
@@ -11172,7 +11180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>20006</v>
       </c>
@@ -11198,7 +11206,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>10577</v>
       </c>
@@ -11224,7 +11232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>8385</v>
       </c>
@@ -11250,7 +11258,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>26745</v>
       </c>
@@ -11276,7 +11284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>35577</v>
       </c>
@@ -11302,7 +11310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>36925</v>
       </c>
@@ -11328,7 +11336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>30126</v>
       </c>
@@ -11354,7 +11362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>19427</v>
       </c>
@@ -11380,7 +11388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>32607</v>
       </c>
@@ -11406,7 +11414,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>32264</v>
       </c>
@@ -11432,7 +11440,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>12557</v>
       </c>
@@ -11458,7 +11466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>2856</v>
       </c>
@@ -11484,7 +11492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>25019</v>
       </c>
@@ -11510,7 +11518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>31792</v>
       </c>
@@ -11536,7 +11544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>26177</v>
       </c>
@@ -11562,7 +11570,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>35833</v>
       </c>
@@ -11588,7 +11596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>16471</v>
       </c>
@@ -11614,7 +11622,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>35592</v>
       </c>
@@ -11640,7 +11648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>36308</v>
       </c>
@@ -11666,7 +11674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>9530</v>
       </c>
@@ -11692,7 +11700,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>29208</v>
       </c>
@@ -11718,7 +11726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>7012</v>
       </c>
@@ -11744,7 +11752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>30475</v>
       </c>
@@ -11770,7 +11778,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>35288</v>
       </c>
@@ -11796,7 +11804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>32533</v>
       </c>
@@ -11822,7 +11830,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>18881</v>
       </c>
@@ -11848,7 +11856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>35024</v>
       </c>
@@ -11874,7 +11882,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>26052</v>
       </c>
@@ -11900,7 +11908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>596</v>
       </c>
@@ -11926,7 +11934,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>30773</v>
       </c>
@@ -11952,7 +11960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>26368</v>
       </c>
@@ -11978,7 +11986,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>31707</v>
       </c>
@@ -12004,7 +12012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>31308</v>
       </c>
@@ -12030,7 +12038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>32939</v>
       </c>
@@ -12056,7 +12064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>5774</v>
       </c>
@@ -12082,7 +12090,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>34437</v>
       </c>
@@ -12108,7 +12116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>1507</v>
       </c>
@@ -12134,7 +12142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>36347</v>
       </c>
@@ -12160,7 +12168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>32875</v>
       </c>
@@ -12186,7 +12194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>14999</v>
       </c>
@@ -12212,7 +12220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>357</v>
       </c>
@@ -12238,7 +12246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>5586</v>
       </c>
@@ -12264,7 +12272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>34782</v>
       </c>
@@ -12290,7 +12298,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>4033</v>
       </c>
@@ -12316,7 +12324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>33023</v>
       </c>
@@ -12342,7 +12350,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>31037</v>
       </c>
@@ -12368,7 +12376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>29571</v>
       </c>
@@ -12394,7 +12402,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>33780</v>
       </c>
@@ -12420,7 +12428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>5819</v>
       </c>
@@ -12446,7 +12454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>31600</v>
       </c>
@@ -12472,7 +12480,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>27261</v>
       </c>
@@ -12498,7 +12506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>6502</v>
       </c>
@@ -12524,7 +12532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>36826</v>
       </c>
@@ -12550,7 +12558,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>36520</v>
       </c>
@@ -12576,7 +12584,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>20695</v>
       </c>
@@ -12602,7 +12610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>35384</v>
       </c>
@@ -12628,7 +12636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>12396</v>
       </c>
@@ -12654,7 +12662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>15419</v>
       </c>
@@ -12680,7 +12688,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>17946</v>
       </c>
@@ -12706,7 +12714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>2142</v>
       </c>
@@ -12732,7 +12740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>29953</v>
       </c>
@@ -12758,7 +12766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>1673</v>
       </c>
@@ -12784,7 +12792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>25060</v>
       </c>
@@ -12810,7 +12818,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>8027</v>
       </c>
@@ -12836,7 +12844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>32458</v>
       </c>
@@ -12862,7 +12870,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>4937</v>
       </c>
@@ -12888,7 +12896,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>11827</v>
       </c>
@@ -12914,7 +12922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>29550</v>
       </c>
@@ -12940,7 +12948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>16389</v>
       </c>
@@ -12966,7 +12974,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>22094</v>
       </c>
@@ -12992,7 +13000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>12820</v>
       </c>
@@ -13018,7 +13026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>2832</v>
       </c>
@@ -13044,7 +13052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>31754</v>
       </c>
@@ -13070,7 +13078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>23893</v>
       </c>
@@ -13096,7 +13104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>25032</v>
       </c>
@@ -13122,7 +13130,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>17094</v>
       </c>
@@ -13148,7 +13156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>36270</v>
       </c>
@@ -13174,7 +13182,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>34932</v>
       </c>
@@ -13200,7 +13208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>14077</v>
       </c>
@@ -13226,7 +13234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>24969</v>
       </c>
@@ -13252,7 +13260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>5832</v>
       </c>
@@ -13278,7 +13286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>11989</v>
       </c>
@@ -13304,7 +13312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>25126</v>
       </c>
@@ -13330,7 +13338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>2037</v>
       </c>
@@ -13356,7 +13364,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>8109</v>
       </c>
@@ -13382,7 +13390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>36678</v>
       </c>
@@ -13408,7 +13416,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>6670</v>
       </c>
@@ -13434,7 +13442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>23658</v>
       </c>
@@ -13460,7 +13468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>35195</v>
       </c>
@@ -13486,7 +13494,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>5369</v>
       </c>
@@ -13512,7 +13520,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>2632</v>
       </c>
@@ -13538,7 +13546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>32498</v>
       </c>
@@ -13564,7 +13572,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>18679</v>
       </c>
@@ -13590,7 +13598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>3501</v>
       </c>
@@ -13616,7 +13624,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>35176</v>
       </c>
@@ -13642,7 +13650,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>36863</v>
       </c>
@@ -13668,7 +13676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>447</v>
       </c>
@@ -13694,7 +13702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>36724</v>
       </c>
@@ -13720,7 +13728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>36747</v>
       </c>
@@ -13746,7 +13754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>16950</v>
       </c>
@@ -13772,7 +13780,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>4514</v>
       </c>
@@ -13798,7 +13806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>11151</v>
       </c>
@@ -13824,7 +13832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>22115</v>
       </c>
@@ -13850,7 +13858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>2788</v>
       </c>
@@ -13876,7 +13884,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>23946</v>
       </c>
@@ -13902,7 +13910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>29855</v>
       </c>
@@ -13928,7 +13936,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>12135</v>
       </c>
@@ -13954,7 +13962,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>35227</v>
       </c>
@@ -13980,7 +13988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>19680</v>
       </c>
@@ -14006,7 +14014,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>31070</v>
       </c>
@@ -14032,7 +14040,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>21559</v>
       </c>
@@ -14058,7 +14066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>24135</v>
       </c>
@@ -14084,7 +14092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>14551</v>
       </c>
@@ -14110,7 +14118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>17457</v>
       </c>
@@ -14136,7 +14144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>24290</v>
       </c>
@@ -14162,7 +14170,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>27571</v>
       </c>
@@ -14188,7 +14196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
         <v>16745</v>
       </c>
@@ -14214,7 +14222,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>35414</v>
       </c>
@@ -14240,7 +14248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
         <v>8370</v>
       </c>
@@ -14266,7 +14274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>1622</v>
       </c>
@@ -14292,7 +14300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
         <v>34165</v>
       </c>
@@ -14318,7 +14326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>32157</v>
       </c>
@@ -14344,7 +14352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
         <v>34279</v>
       </c>
@@ -14370,7 +14378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>35964</v>
       </c>
@@ -14396,7 +14404,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
         <v>33682</v>
       </c>
@@ -14422,7 +14430,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>28641</v>
       </c>
@@ -14448,7 +14456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
         <v>12671</v>
       </c>
@@ -14474,7 +14482,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>7349</v>
       </c>
@@ -14500,7 +14508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
         <v>5066</v>
       </c>
@@ -14526,7 +14534,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>30585</v>
       </c>
@@ -14552,7 +14560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
         <v>1838</v>
       </c>
@@ -14578,7 +14586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>36578</v>
       </c>
@@ -14604,7 +14612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>29591</v>
       </c>
@@ -14630,7 +14638,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>34916</v>
       </c>
@@ -14656,7 +14664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
         <v>7085</v>
       </c>
@@ -14682,7 +14690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>33627</v>
       </c>
@@ -14708,7 +14716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
         <v>28831</v>
       </c>
@@ -14734,7 +14742,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>10483</v>
       </c>
@@ -14760,7 +14768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
         <v>34780</v>
       </c>
@@ -14786,7 +14794,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>17596</v>
       </c>
@@ -14812,7 +14820,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
         <v>24000</v>
       </c>
@@ -14838,7 +14846,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>27231</v>
       </c>
@@ -14864,7 +14872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
         <v>2453</v>
       </c>
@@ -14890,7 +14898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>36396</v>
       </c>
@@ -14916,7 +14924,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
         <v>3709</v>
       </c>
@@ -14942,7 +14950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>1349</v>
       </c>
@@ -14968,7 +14976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
         <v>36644</v>
       </c>
@@ -14994,7 +15002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>19207</v>
       </c>
@@ -15020,7 +15028,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
         <v>20111</v>
       </c>
@@ -15046,7 +15054,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>554</v>
       </c>
@@ -15072,7 +15080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>1155</v>
       </c>
@@ -15098,7 +15106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>5051</v>
       </c>
@@ -15124,7 +15132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
         <v>9153</v>
       </c>
@@ -15150,7 +15158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>25223</v>
       </c>
@@ -15176,7 +15184,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
         <v>28793</v>
       </c>
@@ -15202,7 +15210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>6881</v>
       </c>
@@ -15228,7 +15236,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A274" s="2">
         <v>10031</v>
       </c>
@@ -15254,7 +15262,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>985</v>
       </c>
@@ -15280,7 +15288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A276" s="2">
         <v>28853</v>
       </c>
@@ -15306,7 +15314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>36310</v>
       </c>
@@ -15332,7 +15340,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A278" s="2">
         <v>5612</v>
       </c>
@@ -15358,7 +15366,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>35173</v>
       </c>
@@ -15384,7 +15392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" s="2">
         <v>25763</v>
       </c>
@@ -15410,7 +15418,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>36551</v>
       </c>
@@ -15436,7 +15444,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" s="2">
         <v>33816</v>
       </c>
@@ -15462,7 +15470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>35320</v>
       </c>
@@ -15488,7 +15496,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" s="2">
         <v>28565</v>
       </c>
@@ -15514,7 +15522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>30446</v>
       </c>
@@ -15540,7 +15548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" s="2">
         <v>16333</v>
       </c>
@@ -15566,7 +15574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>20791</v>
       </c>
@@ -15592,7 +15600,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" s="2">
         <v>35906</v>
       </c>
@@ -15618,7 +15626,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" s="3">
         <v>34217</v>
       </c>
@@ -15644,7 +15652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" s="2">
         <v>21621</v>
       </c>
@@ -15670,7 +15678,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" s="3">
         <v>6854</v>
       </c>
@@ -15696,7 +15704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A292" s="2">
         <v>30526</v>
       </c>
@@ -15722,7 +15730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
         <v>25410</v>
       </c>
@@ -15748,7 +15756,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" s="2">
         <v>30338</v>
       </c>
@@ -15774,7 +15782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="295" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A295" s="3">
         <v>34879</v>
       </c>
@@ -15800,7 +15808,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A296" s="2">
         <v>2436</v>
       </c>
@@ -15826,7 +15834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" s="3">
         <v>5731</v>
       </c>
@@ -15852,7 +15860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="298" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" s="2">
         <v>15901</v>
       </c>
@@ -15878,7 +15886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
         <v>7521</v>
       </c>
@@ -15904,7 +15912,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="300" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A300" s="2">
         <v>22266</v>
       </c>
@@ -15930,7 +15938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A301" s="3">
         <v>29672</v>
       </c>
@@ -15956,7 +15964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="302" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A302" s="2">
         <v>32848</v>
       </c>
@@ -15982,7 +15990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="303" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A303" s="3">
         <v>7829</v>
       </c>
@@ -16008,7 +16016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A304" s="2">
         <v>9300</v>
       </c>
@@ -16034,7 +16042,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="305" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A305" s="3">
         <v>16633</v>
       </c>
@@ -16060,7 +16068,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>35468</v>
       </c>
@@ -16086,7 +16094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="307" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A307" s="3">
         <v>11333</v>
       </c>
@@ -16112,7 +16120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>21531</v>
       </c>
@@ -16138,7 +16146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="309" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A309" s="3">
         <v>13564</v>
       </c>
@@ -16164,7 +16172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A310" s="2">
         <v>36092</v>
       </c>
@@ -16190,7 +16198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="311" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A311" s="3">
         <v>17885</v>
       </c>
@@ -16216,7 +16224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" s="2">
         <v>9945</v>
       </c>
@@ -16242,7 +16250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A313" s="3">
         <v>35636</v>
       </c>
@@ -16268,7 +16276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="314" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A314" s="2">
         <v>24518</v>
       </c>
@@ -16294,7 +16302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A315" s="3">
         <v>30345</v>
       </c>
@@ -16320,7 +16328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A316" s="2">
         <v>35099</v>
       </c>
@@ -16346,7 +16354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="317" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A317" s="3">
         <v>31701</v>
       </c>
@@ -16372,7 +16380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="318" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>35409</v>
       </c>
@@ -16398,7 +16406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A319" s="3">
         <v>32924</v>
       </c>
@@ -16424,7 +16432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="320" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>36864</v>
       </c>
@@ -16450,7 +16458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="321" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A321" s="3">
         <v>36947</v>
       </c>
@@ -16476,7 +16484,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="322" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A322" s="2">
         <v>31779</v>
       </c>
@@ -16502,7 +16510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323" s="3">
         <v>31273</v>
       </c>
@@ -16528,7 +16536,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324" s="2">
         <v>35252</v>
       </c>
@@ -16554,7 +16562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325" s="3">
         <v>35568</v>
       </c>
@@ -16580,7 +16588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A326" s="2">
         <v>36568</v>
       </c>
@@ -16606,7 +16614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A327" s="3">
         <v>36632</v>
       </c>
@@ -16632,7 +16640,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="328" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A328" s="2">
         <v>35124</v>
       </c>
@@ -16658,7 +16666,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="329" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A329" s="3">
         <v>12230</v>
       </c>
@@ -16684,7 +16692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="330" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A330" s="2">
         <v>30024</v>
       </c>
@@ -16710,7 +16718,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="331" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A331" s="3">
         <v>30736</v>
       </c>
@@ -16736,7 +16744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="332" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>24028</v>
       </c>
@@ -16762,7 +16770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="333" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A333" s="3">
         <v>27721</v>
       </c>
@@ -16788,7 +16796,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334" s="2">
         <v>34176</v>
       </c>
@@ -16814,7 +16822,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="335" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A335" s="3">
         <v>12505</v>
       </c>
@@ -16840,7 +16848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A336" s="2">
         <v>7694</v>
       </c>
@@ -16866,7 +16874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="337" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" s="3">
         <v>6557</v>
       </c>
@@ -16892,7 +16900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="338" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
         <v>892</v>
       </c>
@@ -16918,7 +16926,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="339" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A339" s="3">
         <v>26244</v>
       </c>
@@ -16944,7 +16952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="340" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>31704</v>
       </c>
@@ -16970,7 +16978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A341" s="3">
         <v>23742</v>
       </c>
@@ -16996,7 +17004,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="342" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A342" s="2">
         <v>14051</v>
       </c>
@@ -17022,7 +17030,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="343" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A343" s="3">
         <v>30608</v>
       </c>
@@ -17048,7 +17056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
         <v>25437</v>
       </c>
@@ -17074,7 +17082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A345" s="3">
         <v>31331</v>
       </c>
@@ -17100,7 +17108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="346" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <v>11401</v>
       </c>
@@ -17126,7 +17134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
         <v>14055</v>
       </c>
@@ -17152,7 +17160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <v>28691</v>
       </c>
@@ -17178,7 +17186,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="349" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A349" s="3">
         <v>32975</v>
       </c>
@@ -17204,7 +17212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="350" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <v>31826</v>
       </c>
@@ -17230,7 +17238,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="351" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A351" s="3">
         <v>31590</v>
       </c>
@@ -17256,7 +17264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="352" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <v>7813</v>
       </c>
@@ -17282,7 +17290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="353" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A353" s="3">
         <v>23708</v>
       </c>
@@ -17308,7 +17316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="354" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <v>9764</v>
       </c>
@@ -17334,7 +17342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A355" s="3">
         <v>12021</v>
       </c>
@@ -17360,7 +17368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="356" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A356" s="2">
         <v>31556</v>
       </c>
@@ -17386,7 +17394,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="357" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A357" s="3">
         <v>31095</v>
       </c>
@@ -17412,7 +17420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" s="2">
         <v>2104</v>
       </c>
@@ -17438,7 +17446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="359" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" s="3">
         <v>19387</v>
       </c>
@@ -17464,7 +17472,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A360" s="2">
         <v>1578</v>
       </c>
@@ -17490,7 +17498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A361" s="3">
         <v>24984</v>
       </c>
@@ -17516,7 +17524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A362" s="2">
         <v>16813</v>
       </c>
@@ -17542,7 +17550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A363" s="3">
         <v>17385</v>
       </c>
@@ -17568,7 +17576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="364" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A364" s="2">
         <v>13473</v>
       </c>
@@ -17594,7 +17602,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A365" s="3">
         <v>1297</v>
       </c>
@@ -17620,7 +17628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="366" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A366" s="2">
         <v>8908</v>
       </c>
@@ -17646,7 +17654,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="367" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A367" s="3">
         <v>20253</v>
       </c>
@@ -17672,7 +17680,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A368" s="2">
         <v>16294</v>
       </c>
@@ -17698,7 +17706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="369" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A369" s="3">
         <v>17277</v>
       </c>
@@ -17724,7 +17732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="370" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A370" s="2">
         <v>26629</v>
       </c>
@@ -17750,7 +17758,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A371" s="3">
         <v>26058</v>
       </c>
@@ -17776,7 +17784,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A372" s="2">
         <v>6138</v>
       </c>
@@ -17802,7 +17810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="373" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A373" s="3">
         <v>13667</v>
       </c>
@@ -17828,7 +17836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="374" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A374" s="2">
         <v>11430</v>
       </c>
@@ -17854,7 +17862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="375" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A375" s="3">
         <v>24637</v>
       </c>
@@ -17880,7 +17888,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A376" s="2">
         <v>27039</v>
       </c>
@@ -17906,7 +17914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A377" s="3">
         <v>25385</v>
       </c>
@@ -17932,7 +17940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A378" s="2">
         <v>12487</v>
       </c>
@@ -17958,7 +17966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="379" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A379" s="3">
         <v>17404</v>
       </c>
@@ -17984,7 +17992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="380" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A380" s="2">
         <v>163</v>
       </c>
@@ -18010,7 +18018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="381" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A381" s="3">
         <v>3458</v>
       </c>
@@ -18036,7 +18044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A382" s="2">
         <v>23458</v>
       </c>
@@ -18062,7 +18070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A383" s="3">
         <v>3960</v>
       </c>
@@ -18088,7 +18096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="384" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A384" s="2">
         <v>1802</v>
       </c>
@@ -18114,7 +18122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="385" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A385" s="3">
         <v>9036</v>
       </c>
@@ -18140,7 +18148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A386" s="2">
         <v>22930</v>
       </c>
@@ -18166,7 +18174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="387" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A387" s="3">
         <v>8367</v>
       </c>
@@ -18192,7 +18200,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="388" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A388" s="2">
         <v>8394</v>
       </c>
@@ -18218,7 +18226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="389" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A389" s="3">
         <v>21882</v>
       </c>
@@ -18244,7 +18252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A390" s="2">
         <v>16198</v>
       </c>
@@ -18270,7 +18278,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="391" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A391" s="3">
         <v>17417</v>
       </c>
@@ -18296,7 +18304,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="392" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A392" s="2">
         <v>22459</v>
       </c>
@@ -18322,7 +18330,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="393" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A393" s="3">
         <v>2653</v>
       </c>
@@ -18348,7 +18356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="394" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A394" s="2">
         <v>20584</v>
       </c>
@@ -18374,7 +18382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="395" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A395" s="3">
         <v>9391</v>
       </c>
@@ -18400,7 +18408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="396" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A396" s="2">
         <v>11612</v>
       </c>
@@ -18426,7 +18434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A397" s="3">
         <v>21988</v>
       </c>
@@ -18452,7 +18460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A398" s="2">
         <v>12537</v>
       </c>
@@ -18478,7 +18486,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="399" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A399" s="3">
         <v>21326</v>
       </c>
@@ -18504,7 +18512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="400" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A400" s="2">
         <v>18741</v>
       </c>
@@ -18530,7 +18538,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="401" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A401" s="3">
         <v>11208</v>
       </c>
@@ -18556,7 +18564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="402" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A402" s="2">
         <v>18260</v>
       </c>
@@ -18582,7 +18590,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A403" s="3">
         <v>7191</v>
       </c>
@@ -18608,7 +18616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="404" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A404" s="2">
         <v>12722</v>
       </c>
@@ -18634,7 +18642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="405" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A405" s="3">
         <v>12267</v>
       </c>
@@ -18660,7 +18668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="406" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A406" s="2">
         <v>15208</v>
       </c>
@@ -18686,7 +18694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="407" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A407" s="3">
         <v>7427</v>
       </c>
@@ -18712,7 +18720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="408" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A408" s="2">
         <v>16952</v>
       </c>
@@ -18738,7 +18746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A409" s="3">
         <v>17433</v>
       </c>
@@ -18764,7 +18772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="410" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A410" s="2">
         <v>1298</v>
       </c>
@@ -18790,7 +18798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="411" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A411" s="3">
         <v>17504</v>
       </c>
@@ -18816,7 +18824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A412" s="2">
         <v>11533</v>
       </c>
@@ -18842,7 +18850,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="413" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A413" s="3">
         <v>16193</v>
       </c>
@@ -18868,7 +18876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="414" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A414" s="2">
         <v>13127</v>
       </c>
@@ -18894,7 +18902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A415" s="3">
         <v>11641</v>
       </c>
@@ -18920,7 +18928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="416" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A416" s="2">
         <v>270</v>
       </c>
@@ -18946,7 +18954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A417" s="3">
         <v>12088</v>
       </c>
@@ -18972,7 +18980,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="418" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A418" s="2">
         <v>5910</v>
       </c>
@@ -18998,7 +19006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="419" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A419" s="3">
         <v>10263</v>
       </c>
@@ -19024,7 +19032,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="420" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A420" s="2">
         <v>12367</v>
       </c>
@@ -19050,7 +19058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A421" s="3">
         <v>13934</v>
       </c>
@@ -19076,7 +19084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="422" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A422" s="2">
         <v>5935</v>
       </c>
@@ -19102,7 +19110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="423" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A423" s="3">
         <v>1511</v>
       </c>
@@ -19128,7 +19136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A424" s="2">
         <v>13827</v>
       </c>
@@ -19154,7 +19162,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="425" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A425" s="3">
         <v>7140</v>
       </c>
@@ -19180,7 +19188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="426" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A426" s="2">
         <v>11046</v>
       </c>
@@ -19206,7 +19214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="427" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A427" s="3">
         <v>6182</v>
       </c>
@@ -19232,7 +19240,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="428" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A428" s="2">
         <v>3465</v>
       </c>
@@ -19258,7 +19266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="429" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A429" s="3">
         <v>11719</v>
       </c>
@@ -19284,7 +19292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="430" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A430" s="2">
         <v>8672</v>
       </c>
@@ -19310,7 +19318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="431" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A431" s="3">
         <v>12520</v>
       </c>
@@ -19336,7 +19344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="432" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A432" s="2">
         <v>9093</v>
       </c>
@@ -19362,7 +19370,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A433" s="3">
         <v>847</v>
       </c>
@@ -19388,7 +19396,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="434" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A434" s="2">
         <v>1608</v>
       </c>
@@ -19414,7 +19422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="435" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A435" s="3">
         <v>7824</v>
       </c>
@@ -19440,7 +19448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="436" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A436" s="2">
         <v>7304</v>
       </c>
@@ -19466,7 +19474,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="437" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A437" s="3">
         <v>1751</v>
       </c>
@@ -19492,7 +19500,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="438" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A438" s="2">
         <v>7504</v>
       </c>
@@ -19518,7 +19526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="439" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" ht="65" x14ac:dyDescent="0.2">
       <c r="A439" s="3">
         <v>5177</v>
       </c>
@@ -19544,7 +19552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="440" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" ht="52" x14ac:dyDescent="0.2">
       <c r="A440" s="2">
         <v>1679</v>
       </c>
@@ -19570,7 +19578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="441" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A441" s="3">
         <v>3466</v>
       </c>
@@ -19596,7 +19604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="442" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A442" s="2">
         <v>3445</v>
       </c>
@@ -19622,7 +19630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A443" s="3">
         <v>713</v>
       </c>
@@ -19648,7 +19656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A444" s="2">
         <v>1248</v>
       </c>
@@ -19674,7 +19682,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A445" s="3">
         <v>4096</v>
       </c>
@@ -19700,7 +19708,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="446" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A446" s="2">
         <v>2838</v>
       </c>
@@ -19726,7 +19734,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="447" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A447" s="3">
         <v>2088</v>
       </c>
@@ -19752,7 +19760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="448" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A448" s="2">
         <v>1928</v>
       </c>
@@ -19778,7 +19786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="449" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A449" s="3">
         <v>1900</v>
       </c>
@@ -19804,7 +19812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="450" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8" ht="39" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
         <v>1446</v>
       </c>
@@ -19830,7 +19838,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A451" s="3">
         <v>3958</v>
       </c>
@@ -19856,7 +19864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="452" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A452" s="2">
         <v>3626</v>
       </c>
@@ -19882,7 +19890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A453" s="3">
         <v>644</v>
       </c>
@@ -19908,7 +19916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="454" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A454" s="2">
         <v>3223</v>
       </c>
@@ -19934,7 +19942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="455" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A455" s="3">
         <v>2215</v>
       </c>
@@ -19960,7 +19968,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A456" s="2">
         <v>629</v>
       </c>
@@ -19986,7 +19994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="457" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A457" s="3">
         <v>216</v>
       </c>

</xml_diff>